<commit_message>
Change in data and column
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -11,16 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Gum</t>
   </si>
@@ -32,22 +23,22 @@
   </si>
   <si>
     <t>Hot Chips</t>
+  </si>
+  <si>
+    <t>Carrots</t>
+  </si>
+  <si>
+    <t>Cake</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -71,14 +62,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -301,54 +289,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="B4" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>25.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
-        <v>21.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B6" s="1">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>